<commit_message>
Added Excel details - Add Clients
</commit_message>
<xml_diff>
--- a/src/main/java/testData/HoursheetsTestData.xlsx
+++ b/src/main/java/testData/HoursheetsTestData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="9540" windowHeight="6420" tabRatio="500"/>
+    <workbookView windowWidth="18530" windowHeight="7070" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="clients" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>firstname</t>
   </si>
@@ -33,7 +33,7 @@
     <t>country</t>
   </si>
   <si>
-    <t>phone</t>
+    <t>phoneNo</t>
   </si>
   <si>
     <t>countrycode</t>
@@ -58,6 +58,30 @@
   </si>
   <si>
     <t>Devtest123@</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>fax</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>FName 4</t>
+  </si>
+  <si>
+    <t>LName 4</t>
+  </si>
+  <si>
+    <t>devtest.4@mexcool2.co</t>
+  </si>
+  <si>
+    <t>25 George sreet, Downing town, Pennnsylvania</t>
+  </si>
+  <si>
+    <t>https://greatdeas.ae</t>
   </si>
 </sst>
 </file>
@@ -65,10 +89,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -95,42 +119,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -139,17 +127,60 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,6 +194,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -171,34 +225,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -210,29 +256,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,181 +291,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,47 +600,47 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -625,102 +649,117 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1057,68 +1096,68 @@
   <sheetPr/>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="2" width="11" style="2"/>
-    <col min="3" max="3" width="23.8333333333333" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11" style="2"/>
-    <col min="5" max="5" width="14.5833333333333" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.5833333333333" style="2"/>
-    <col min="7" max="7" width="15" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.1666666666667" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11" style="3"/>
+    <col min="1" max="2" width="11" style="7"/>
+    <col min="3" max="3" width="23.8333333333333" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11" style="7"/>
+    <col min="5" max="5" width="14.5833333333333" style="7" customWidth="1"/>
+    <col min="6" max="6" width="11.5833333333333" style="7"/>
+    <col min="7" max="7" width="15" style="7" customWidth="1"/>
+    <col min="8" max="8" width="16.1666666666667" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="11" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:8">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="6" customFormat="1" spans="1:8">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="7">
         <v>5550123432</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1134,14 +1173,73 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" outlineLevelRow="1" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="2" width="11" style="2"/>
+    <col min="3" max="3" width="22" style="2" customWidth="1"/>
+    <col min="4" max="4" width="33.0833333333333" style="2" customWidth="1"/>
+    <col min="5" max="6" width="11" style="2"/>
+    <col min="7" max="7" width="22.0833333333333" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="11" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" ht="31" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2">
+        <v>98398198</v>
+      </c>
+      <c r="F2" s="2">
+        <v>31879381</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="devtest.4@mexcool2.co" tooltip="mailto:devtest.4@mexcool2.co"/>
+    <hyperlink ref="G2" r:id="rId2" display="https://greatdeas.ae"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Add Invoice - Added
</commit_message>
<xml_diff>
--- a/src/main/java/testData/HoursheetsTestData.xlsx
+++ b/src/main/java/testData/HoursheetsTestData.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="18530" windowHeight="7070" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" r:id="rId1"/>
     <sheet name="clients" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="invoice" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>firstname</t>
   </si>
@@ -82,6 +82,78 @@
   </si>
   <si>
     <t>https://greatdeas.ae</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>PricePerUnit</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Work 1</t>
+  </si>
+  <si>
+    <t>This describes  the work billed for work 1</t>
+  </si>
+  <si>
+    <t>Work 2</t>
+  </si>
+  <si>
+    <t>This describes  the work billed for work 2</t>
+  </si>
+  <si>
+    <t>Work 3</t>
+  </si>
+  <si>
+    <t>This describes  the work billed for work 3</t>
+  </si>
+  <si>
+    <t>Work 4</t>
+  </si>
+  <si>
+    <t>This describes  the work billed for work 4</t>
+  </si>
+  <si>
+    <t>Work 5</t>
+  </si>
+  <si>
+    <t>This describes  the work billed for work 5</t>
+  </si>
+  <si>
+    <t>Work 6</t>
+  </si>
+  <si>
+    <t>This describes  the work billed for work 6</t>
+  </si>
+  <si>
+    <t>Work 7</t>
+  </si>
+  <si>
+    <t>This describes  the work billed for work 7</t>
+  </si>
+  <si>
+    <t>Work 8</t>
+  </si>
+  <si>
+    <t>This describes  the work billed for work 8</t>
+  </si>
+  <si>
+    <t>Work 9</t>
+  </si>
+  <si>
+    <t>This describes  the work billed for work 9</t>
+  </si>
+  <si>
+    <t>Work 10</t>
+  </si>
+  <si>
+    <t>This describes  the work billed for work 10</t>
   </si>
 </sst>
 </file>
@@ -89,9 +161,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -130,57 +202,57 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -195,6 +267,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -225,46 +312,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -291,85 +363,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,97 +537,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,26 +572,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -566,23 +629,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -597,161 +654,180 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
@@ -1102,62 +1178,62 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="2" width="11" style="7"/>
-    <col min="3" max="3" width="23.8333333333333" style="7" customWidth="1"/>
-    <col min="4" max="4" width="11" style="7"/>
-    <col min="5" max="5" width="14.5833333333333" style="7" customWidth="1"/>
-    <col min="6" max="6" width="11.5833333333333" style="7"/>
-    <col min="7" max="7" width="15" style="7" customWidth="1"/>
-    <col min="8" max="8" width="16.1666666666667" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="11" style="8"/>
+    <col min="1" max="2" width="11" style="9"/>
+    <col min="3" max="3" width="23.8333333333333" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11" style="9"/>
+    <col min="5" max="5" width="14.5833333333333" style="9" customWidth="1"/>
+    <col min="6" max="6" width="11.5833333333333" style="9"/>
+    <col min="7" max="7" width="15" style="9" customWidth="1"/>
+    <col min="8" max="8" width="16.1666666666667" style="9" customWidth="1"/>
+    <col min="9" max="16384" width="11" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:8">
-      <c r="A1" s="9" t="s">
+    <row r="1" s="8" customFormat="1" spans="1:8">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="9">
         <v>5550123432</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1175,18 +1251,18 @@
   <sheetPr/>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="2" width="11" style="2"/>
-    <col min="3" max="3" width="22" style="2" customWidth="1"/>
-    <col min="4" max="4" width="33.0833333333333" style="2" customWidth="1"/>
-    <col min="5" max="6" width="11" style="2"/>
-    <col min="7" max="7" width="22.0833333333333" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="11" style="2"/>
+    <col min="1" max="2" width="11" style="5"/>
+    <col min="3" max="3" width="22" style="5" customWidth="1"/>
+    <col min="4" max="4" width="33.0833333333333" style="5" customWidth="1"/>
+    <col min="5" max="6" width="11" style="5"/>
+    <col min="7" max="7" width="22.0833333333333" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="11" style="5"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
@@ -1213,25 +1289,25 @@
       </c>
     </row>
     <row r="2" ht="31" spans="1:7">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="5">
         <v>98398198</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="5">
         <v>31879381</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1248,14 +1324,175 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="11" style="2"/>
+    <col min="2" max="2" width="34.8333333333333" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.5833333333333" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="11" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4">
+        <v>21.01</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" spans="1:4">
+      <c r="A3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="4">
+        <v>22.02</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="4">
+        <v>23.03</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4">
+        <v>24.04</v>
+      </c>
+      <c r="D5" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" spans="1:4">
+      <c r="A6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="4">
+        <v>25.05</v>
+      </c>
+      <c r="D6" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="1" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4">
+        <v>26.6</v>
+      </c>
+      <c r="D7" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" s="2" customFormat="1" spans="1:4">
+      <c r="A8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="4">
+        <v>27.7</v>
+      </c>
+      <c r="D8" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" s="2" customFormat="1" spans="1:4">
+      <c r="A9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="4">
+        <v>28.8</v>
+      </c>
+      <c r="D9" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="1" spans="1:4">
+      <c r="A10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="4">
+        <v>29.9</v>
+      </c>
+      <c r="D10" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" s="2" customFormat="1" spans="1:4">
+      <c r="A11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="4">
+        <v>30.2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Edit clients - Added
</commit_message>
<xml_diff>
--- a/src/main/java/testData/HoursheetsTestData.xlsx
+++ b/src/main/java/testData/HoursheetsTestData.xlsx
@@ -9,14 +9,16 @@
   <sheets>
     <sheet name="signup" sheetId="1" r:id="rId1"/>
     <sheet name="clients" sheetId="2" r:id="rId2"/>
-    <sheet name="invoice" sheetId="3" r:id="rId3"/>
+    <sheet name="editClients" sheetId="5" r:id="rId3"/>
+    <sheet name="invoice" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>firstname</t>
   </si>
@@ -82,6 +84,15 @@
   </si>
   <si>
     <t>https://greatdeas.ae</t>
+  </si>
+  <si>
+    <t>EdFName 4</t>
+  </si>
+  <si>
+    <t>EdLName 4</t>
+  </si>
+  <si>
+    <t>devtest.456@mexcool2.co</t>
   </si>
   <si>
     <t>Item</t>
@@ -161,9 +172,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -200,27 +211,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -236,7 +226,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -252,6 +263,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -267,7 +286,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -282,61 +333,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,19 +374,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,13 +506,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -405,43 +530,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,97 +542,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -583,6 +594,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -628,24 +663,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -655,163 +672,157 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1324,9 +1335,84 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" outlineLevelRow="1" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="2" width="11" style="5"/>
+    <col min="3" max="3" width="22" style="5" customWidth="1"/>
+    <col min="4" max="4" width="33.0833333333333" style="5" customWidth="1"/>
+    <col min="5" max="6" width="11.5833333333333" style="5"/>
+    <col min="7" max="7" width="22.0833333333333" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="11" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" ht="31" spans="1:7">
+      <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="5">
+        <v>3131313455</v>
+      </c>
+      <c r="F2" s="5">
+        <v>3187973381</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="devtest.456@mexcool2.co" tooltip="mailto:devtest.456@mexcool2.co"/>
+    <hyperlink ref="G2" r:id="rId2" display="https://greatdeas.ae"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1340,24 +1426,24 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4">
         <v>21.01</v>
@@ -1368,10 +1454,10 @@
     </row>
     <row r="3" s="2" customFormat="1" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4">
         <v>22.02</v>
@@ -1382,10 +1468,10 @@
     </row>
     <row r="4" s="2" customFormat="1" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4">
         <v>23.03</v>
@@ -1396,10 +1482,10 @@
     </row>
     <row r="5" s="2" customFormat="1" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C5" s="4">
         <v>24.04</v>
@@ -1410,10 +1496,10 @@
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4">
         <v>25.05</v>
@@ -1424,10 +1510,10 @@
     </row>
     <row r="7" s="2" customFormat="1" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4">
         <v>26.6</v>
@@ -1438,10 +1524,10 @@
     </row>
     <row r="8" s="2" customFormat="1" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C8" s="4">
         <v>27.7</v>
@@ -1452,10 +1538,10 @@
     </row>
     <row r="9" s="2" customFormat="1" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C9" s="4">
         <v>28.8</v>
@@ -1466,10 +1552,10 @@
     </row>
     <row r="10" s="2" customFormat="1" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C10" s="4">
         <v>29.9</v>
@@ -1480,10 +1566,10 @@
     </row>
     <row r="11" s="2" customFormat="1" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C11" s="4">
         <v>30.2</v>
@@ -1496,4 +1582,20 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="15.5"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>